<commit_message>
Set offshore wind shareweight for green hydrogen production to 0
</commit_message>
<xml_diff>
--- a/InputData/elec/GHESS/Green Hydrogen Electricity Supply Shareweights.xlsx
+++ b/InputData/elec/GHESS/Green Hydrogen Electricity Supply Shareweights.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MeganMahajan\Documents\eps-us\InputData\elec\TTS\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MeganMahajan\Documents\eps-us\InputData\elec\GHESS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{460419F9-E16A-400F-91E6-BD5553EB796E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A11E51E6-BA89-4879-AFE0-0753A63A9214}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1280,8 +1280,8 @@
   </sheetPr>
   <dimension ref="A1:AE25"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B31" sqref="B31"/>
+    <sheetView topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="B14" sqref="B14:AE15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2624,94 +2624,94 @@
         <v>14</v>
       </c>
       <c r="B15">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C15">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D15">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E15">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F15">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G15">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H15">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I15">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J15">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K15">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L15">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M15">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N15">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O15">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P15">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q15">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R15">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S15">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="T15">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U15">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="V15">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="W15">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="X15">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Y15">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Z15">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AA15">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AB15">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AC15">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AD15">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AE15">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="16" spans="1:31" x14ac:dyDescent="0.25">

</xml_diff>